<commit_message>
add all the links to fetch texts
</commit_message>
<xml_diff>
--- a/cocurricular_competencies.xlsx
+++ b/cocurricular_competencies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rad/Desktop/UNi/proj/EER/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033CC093-1E78-5E41-862E-1EC49B9A2F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281AEAE1-906E-2140-825E-78B8D26F2017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13760" yWindow="760" windowWidth="20800" windowHeight="21580" xr2:uid="{1CFB208A-0F52-DC46-8BE9-EBACDF921171}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
   <si>
     <t>e@UBCV</t>
   </si>
@@ -605,7 +605,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -657,9 +657,7 @@
       <c r="N1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="O1" s="4"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
update the scrape file and update links in data, progresson nlp_label
</commit_message>
<xml_diff>
--- a/cocurricular_competencies.xlsx
+++ b/cocurricular_competencies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rad/Desktop/UNi/proj/EER/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281AEAE1-906E-2140-825E-78B8D26F2017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B560855-BFAA-454C-9123-A7F7C4D5A8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13760" yWindow="760" windowWidth="20800" windowHeight="21580" xr2:uid="{1CFB208A-0F52-DC46-8BE9-EBACDF921171}"/>
   </bookViews>
@@ -170,9 +170,6 @@
     <t>Planning and project managing skills</t>
   </si>
   <si>
-    <t>testing, process mapping, roadmap, project manage, etc.</t>
-  </si>
-  <si>
     <t>Networking skills</t>
   </si>
   <si>
@@ -213,6 +210,9 @@
   </si>
   <si>
     <t>uncertainty, ambiguity, navigation</t>
+  </si>
+  <si>
+    <t>testing, process mapping, roadmap, project manage</t>
   </si>
 </sst>
 </file>
@@ -605,7 +605,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -776,63 +776,63 @@
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
         <v>45</v>
-      </c>
-      <c r="B17" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
         <v>47</v>
-      </c>
-      <c r="B18" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
         <v>49</v>
-      </c>
-      <c r="B19" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" t="s">
         <v>51</v>
-      </c>
-      <c r="B20" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
         <v>53</v>
-      </c>
-      <c r="B21" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s">
         <v>55</v>
-      </c>
-      <c r="B22" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
         <v>57</v>
-      </c>
-      <c r="B23" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add implementation of nlp_label for comptency classification
</commit_message>
<xml_diff>
--- a/cocurricular_competencies.xlsx
+++ b/cocurricular_competencies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rad/Desktop/UNi/proj/EER/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B560855-BFAA-454C-9123-A7F7C4D5A8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DA0C2E-04C6-6C45-846C-4BFF13CFA22E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13760" yWindow="760" windowWidth="20800" windowHeight="21580" xr2:uid="{1CFB208A-0F52-DC46-8BE9-EBACDF921171}"/>
   </bookViews>
@@ -83,9 +83,6 @@
     <t>Entrepreneur types, traits, key behaviours</t>
   </si>
   <si>
-    <t xml:space="preserve">Opportunity Recognition </t>
-  </si>
-  <si>
     <t>opportunity identification, opportunity recognition, need finding, problem identification</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>Legal Issues</t>
   </si>
   <si>
-    <t>legal matters, contracts, intellectual property, copyright,</t>
-  </si>
-  <si>
     <t>Financial Decision Making</t>
   </si>
   <si>
@@ -188,9 +182,6 @@
     <t>risk-tolerant, open, take initiative, enterprising, committed, traits</t>
   </si>
   <si>
-    <t xml:space="preserve">Enterprising Mindset </t>
-  </si>
-  <si>
     <t>curiosity, self-motivated, experimental, confident, competitive, pro-active</t>
   </si>
   <si>
@@ -213,6 +204,15 @@
   </si>
   <si>
     <t>testing, process mapping, roadmap, project manage</t>
+  </si>
+  <si>
+    <t>Opportunity Recognition</t>
+  </si>
+  <si>
+    <t>Enterprising Mindset</t>
+  </si>
+  <si>
+    <t>legal matters, contracts, intellectual property, copyright</t>
   </si>
 </sst>
 </file>
@@ -605,7 +605,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,10 +616,10 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -669,170 +669,170 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
         <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>